<commit_message>
After Cache Performance Results
</commit_message>
<xml_diff>
--- a/nonFunctionalRequirements/performance/resultados.xlsx
+++ b/nonFunctionalRequirements/performance/resultados.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniw\Documents\ECI\ARSW\Teach-me\nonFunctionalRequirements\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A0518D-3AA0-448D-BA88-BC5776A0E61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D162AD6-C767-434F-BB7E-05908CA87EAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C78633FB-6593-4854-A8B8-F097E8CC81DF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Before Cache" sheetId="1" r:id="rId1"/>
+    <sheet name="Before Cache" sheetId="3" r:id="rId1"/>
     <sheet name="After Cache" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>% de Error</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Promedio (ms)</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>Variables de carga</t>
   </si>
   <si>
@@ -56,6 +53,24 @@
   </si>
   <si>
     <t>Número de Peticiones</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Get Classes</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>URL Login</t>
+  </si>
+  <si>
+    <t>URL Get Classes</t>
+  </si>
+  <si>
+    <t>https://teach2-me.herokuapp.com/login</t>
   </si>
 </sst>
 </file>
@@ -107,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -146,11 +161,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -163,10 +193,25 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -178,148 +223,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -346,6 +253,184 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -356,33 +441,10 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -391,19 +453,74 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -459,9 +576,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-CO" sz="1600" b="1"/>
+              <a:rPr lang="es-CO" sz="1800" b="1" i="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
               <a:t>Get Classes By Name</a:t>
             </a:r>
+            <a:endParaRPr lang="es-CO">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -553,24 +681,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Before Cache'!$C$7:$C$11</c:f>
+              <c:f>'Before Cache'!$E$7:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>809</c:v>
+                  <c:v>404</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1030</c:v>
+                  <c:v>411</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1132</c:v>
+                  <c:v>397</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1898</c:v>
+                  <c:v>318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2160</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,493 +706,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-59B9-498D-BDBB-2B70DF714FC6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1712076752"/>
-        <c:axId val="1711679744"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1712076752"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr lang="es-CO" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="44546A"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="es-CO" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="44546A"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:rPr>
-                  <a:t>Número de Peticiones</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr lang="es-CO" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="44546A"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1711679744"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1711679744"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Duración Promedio (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="es-CO" sz="900">
-                  <a:effectLst/>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                <a:lnSpc>
-                  <a:spcPct val="100000"/>
-                </a:lnSpc>
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-                <a:buClrTx/>
-                <a:buSzTx/>
-                <a:buFontTx/>
-                <a:buNone/>
-                <a:tabLst/>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:sysClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1712076752"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-CO" sz="1800" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Get Classes By Name</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-CO">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'After Cache'!$B$7:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'After Cache'!$C$7:$C$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>521</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>538</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>622</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>568</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>586</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C581-4B89-8B51-10DA35ACB0DB}"/>
+              <c16:uniqueId val="{00000000-2D3E-4638-A687-B35694F66E24}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1121,11 +763,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
                     <a:effectLst/>
                   </a:rPr>
                   <a:t>Número de Peticiones</a:t>
                 </a:r>
                 <a:endParaRPr lang="es-CO" sz="900">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
                   <a:effectLst/>
                 </a:endParaRPr>
               </a:p>
@@ -1257,40 +905,19 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
                     <a:effectLst/>
                   </a:rPr>
                   <a:t>Duración Promedio (ms)</a:t>
                 </a:r>
                 <a:endParaRPr lang="es-CO" sz="900">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
                   <a:effectLst/>
                 </a:endParaRPr>
-              </a:p>
-              <a:p>
-                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr>
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
-                    </a:solidFill>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-CO" sz="900"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1423,6 +1050,1394 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO" sz="1800" b="1"/>
+              <a:t>Login And Get Classes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Before Cache'!$B$7:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Before Cache'!$G$7:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2107</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2354</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1887</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DFCA-453A-A8F2-00FD2ACE4DB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1903596463"/>
+        <c:axId val="1307147519"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1903596463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Número de Peticiones</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO" sz="900">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1307147519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1307147519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Duración Promedio (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO" sz="900">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1903596463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO" sz="1800" b="1" i="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Get Classes By Name</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CO">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'After Cache'!$B$7:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'After Cache'!$E$7:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>411</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C581-4B89-8B51-10DA35ACB0DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="508070448"/>
+        <c:axId val="1799492688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="508070448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Número de Peticiones</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO" sz="900">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1799492688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1799492688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Duración Promedio (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO" sz="900">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508070448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO" sz="1800" b="1"/>
+              <a:t>Login And Get Classes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'After Cache'!$B$7:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'After Cache'!$G$7:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2107</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2354</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1887</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E044-4A97-81EC-4FD78566CC5B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1903596463"/>
+        <c:axId val="1307147519"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1903596463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Número de Peticiones</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO" sz="900">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1307147519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1307147519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Duración Promedio (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO" sz="900">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1903596463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1503,6 +2518,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2535,31 +3630,1065 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93229B8A-24DA-49C7-B83F-B1E31B3D2949}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E381656-3575-40C6-A201-C5EA347C9C60}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2573,6 +4702,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D38728A4-24AF-456F-A8D9-F4D7FF95C568}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2580,16 +4747,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2609,6 +4776,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02E3874D-9A42-498A-9189-22D81EE1D339}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2913,237 +5116,483 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2F8125-2EA6-437F-9D9D-DCBA6C6707D1}">
-  <dimension ref="B2:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7933169D-4136-483D-8D51-36C56DF42599}">
+  <dimension ref="B1:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="19"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="15"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="E6" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
+      <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="6">
-        <v>809</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="C7" s="15">
+        <v>1721</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>404</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0</v>
+      </c>
+      <c r="G7" s="29">
+        <f>C7+E7</f>
+        <v>2125</v>
+      </c>
+      <c r="H7" s="2">
+        <f>D7+F7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="12">
         <v>5</v>
       </c>
-      <c r="C8" s="8">
-        <v>1030</v>
-      </c>
-      <c r="D8" s="12">
+      <c r="C8" s="16">
+        <v>1696</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="16">
+        <v>411</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="30">
+        <f t="shared" ref="G8:H11" si="0">C8+E8</f>
+        <v>2107</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="12">
         <v>10</v>
       </c>
-      <c r="C9" s="8">
-        <v>1132</v>
-      </c>
-      <c r="D9" s="12">
+      <c r="C9" s="16">
+        <v>1272</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>397</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="30">
+        <f t="shared" si="0"/>
+        <v>1669</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="B10" s="12">
         <v>15</v>
       </c>
-      <c r="C10" s="8">
-        <v>1898</v>
-      </c>
-      <c r="D10" s="12">
+      <c r="C10" s="16">
+        <v>2036</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>318</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="30">
+        <f t="shared" si="0"/>
+        <v>2354</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
+      <c r="B11" s="13">
         <v>20</v>
       </c>
-      <c r="C11" s="10">
-        <v>2160</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="C11" s="17">
+        <v>1583</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>304</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="31">
+        <f t="shared" si="0"/>
+        <v>1887</v>
+      </c>
+      <c r="H11" s="32">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:H5"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{928D514D-F784-4A10-9A55-6BD6C647BA08}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4D2BBF59-83CA-4C62-B8DE-CD1C99DCA2AF}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{393BA5C2-1C76-45ED-ADE4-C729B79FA08A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AE1524-C8CF-4627-90E9-C5E0B1F9E240}">
-  <dimension ref="B2:J11"/>
+  <dimension ref="B1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="19"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="18"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="E6" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
+      <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="6">
-        <v>521</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="C7" s="15">
+        <v>1721</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>404</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0</v>
+      </c>
+      <c r="G7" s="29">
+        <f>C7+E7</f>
+        <v>2125</v>
+      </c>
+      <c r="H7" s="2">
+        <f>D7+F7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="12">
         <v>5</v>
       </c>
-      <c r="C8" s="8">
-        <v>538</v>
-      </c>
-      <c r="D8" s="12">
+      <c r="C8" s="16">
+        <v>1696</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="16">
+        <v>411</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="30">
+        <f t="shared" ref="G8:G11" si="0">C8+E8</f>
+        <v>2107</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" ref="H8:H11" si="1">D8+F8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="12">
         <v>10</v>
       </c>
-      <c r="C9" s="8">
-        <v>622</v>
-      </c>
-      <c r="D9" s="12">
+      <c r="C9" s="16">
+        <v>1272</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
+        <v>397</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="30">
+        <f t="shared" si="0"/>
+        <v>1669</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="B10" s="12">
         <v>15</v>
       </c>
-      <c r="C10" s="8">
-        <v>568</v>
-      </c>
-      <c r="D10" s="12">
+      <c r="C10" s="16">
+        <v>2036</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>318</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="30">
+        <f t="shared" si="0"/>
+        <v>2354</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
+      <c r="B11" s="13">
         <v>20</v>
       </c>
-      <c r="C11" s="10">
-        <v>586</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="C11" s="17">
+        <v>1583</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>304</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="31">
+        <f t="shared" si="0"/>
+        <v>1887</v>
+      </c>
+      <c r="H11" s="32">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D2:J2"/>
+  <mergeCells count="7">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="D2:H2"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C4:F4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{E494241E-1D17-445F-873D-711ADB861157}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{DC5296F1-243F-4DEC-BB3C-CBF22F392487}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>